<commit_message>
add columns to Data-Variable-Definitions.xlsx
</commit_message>
<xml_diff>
--- a/ref/Data-Variable-Definitions.xlsx
+++ b/ref/Data-Variable-Definitions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xiaoba/Projects/Udacity/ND-Data-Analyst/p4-dand-explore-and-summarize-data/doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xiaoba/Projects/Udacity/dand-p4-explore-summarise-data/ref/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$C$100</definedName>
+  </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="178">
   <si>
     <t>Variable</t>
   </si>
@@ -354,9 +357,6 @@
   </si>
   <si>
     <t>Unique numeric value associated with the loan.</t>
-  </si>
-  <si>
-    <t>LoanOriginalAmount</t>
   </si>
   <si>
     <t>The origination amount of the loan.</t>
@@ -556,6 +556,74 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>CreditGrade</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of inquiries in the past six months at the time the credit profile was pulled.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Monthly payment on revolving accounts at the time the credit profile was pulled.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of accounts delinquent at the time the credit profile was pulled.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of trades that have never been delinquent at the time the credit profile was pulled.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pre charge-off cumulative gross payments made by the borrower on the loan. If the loan has charged off, this value will exclude any recoveries.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of days delinquent. </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>StatedMonthlyIncome</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>The category of the listing that the borrower selected when posting their listing: 0 - Not Available, 1 - Debt Consolidation, 2 - Home Improvement, 3 - Business, 4 - Personal Loan, 5 - Student Use, 6 - Auto, 7- Other, 8 - Baby&amp;Adoption, 9 - Boat, 10 - Cosmetic Procedure, 11 - Engagement Ring, 12 - Green Loans, 13 - Household Expenses, 14 - Large Purchases, 15 - Medical/Dental, 16 - Motorcycle, 17 - RV, 18 - Taxes, 19 - Vacation, 20 - Wedding Loans</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The cycle the loan was charged off. If the loan has not charged off the value will be null. </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ProsperRating (Alpha)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total number of inquiries at the time the credit profile was pulled.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Note</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Character</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID but not unique</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>POSIXct</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">The Credit rating that was assigned at the time the listing went live. </t>
     </r>
@@ -570,51 +638,43 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>CreditGrade</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of inquiries in the past six months at the time the credit profile was pulled.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Monthly payment on revolving accounts at the time the credit profile was pulled.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of accounts delinquent at the time the credit profile was pulled.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of trades that have never been delinquent at the time the credit profile was pulled.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pre charge-off cumulative gross payments made by the borrower on the loan. If the loan has charged off, this value will exclude any recoveries.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of days delinquent. </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>StatedMonthlyIncome</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>The category of the listing that the borrower selected when posting their listing: 0 - Not Available, 1 - Debt Consolidation, 2 - Home Improvement, 3 - Business, 4 - Personal Loan, 5 - Student Use, 6 - Auto, 7- Other, 8 - Baby&amp;Adoption, 9 - Boat, 10 - Cosmetic Procedure, 11 - Engagement Ring, 12 - Green Loans, 13 - Household Expenses, 14 - Large Purchases, 15 - Medical/Dental, 16 - Motorcycle, 17 - RV, 18 - Taxes, 19 - Vacation, 20 - Wedding Loans</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">The cycle the loan was charged off. If the loan has not charged off the value will be null. </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ProsperRating (Alpha)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Total number of inquiries at the time the credit profile was pulled.</t>
+    <t>No Data available between 2009-05-07 and 2009-07-13.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Only available before 2009-05-04. The dataset begins from 2005-11-09.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Factor</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Numeric</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Logical</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Combined</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Needs Cross Validation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Needs Refactor</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Location</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LoanOriginalAmount</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -622,7 +682,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -668,8 +728,24 @@
       <color theme="11"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="19"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -679,12 +755,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -698,12 +768,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -728,17 +808,51 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+  <cellStyles count="13">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1013,755 +1127,1299 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B100"/>
+  <dimension ref="A1:E100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B82" sqref="B82"/>
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="35.83203125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="35.83203125" style="14" customWidth="1"/>
     <col min="2" max="2" width="66.6640625" style="5" customWidth="1"/>
-    <col min="3" max="20" width="17.33203125" style="5" customWidth="1"/>
-    <col min="21" max="16384" width="14.5" style="5"/>
+    <col min="3" max="3" width="17.33203125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" style="16" customWidth="1"/>
+    <col min="5" max="5" width="28.5" style="9" customWidth="1"/>
+    <col min="6" max="19" width="17.33203125" style="5" customWidth="1"/>
+    <col min="20" max="16384" width="14.5" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.15">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A2" s="4" t="s">
+      <c r="C1" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="36" x14ac:dyDescent="0.15">
+      <c r="A2" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A3" s="4" t="s">
+      <c r="C2" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="36" x14ac:dyDescent="0.15">
+      <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.15">
-      <c r="A4" s="6" t="s">
+      <c r="C3" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="54" x14ac:dyDescent="0.15">
-      <c r="A5" s="8" t="s">
-        <v>152</v>
+      <c r="C4" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="D4" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="54" x14ac:dyDescent="0.15">
+      <c r="A5" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.15">
-      <c r="A6" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="D5" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="54" x14ac:dyDescent="0.15">
-      <c r="A7" s="6" t="s">
+      <c r="C6" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D6" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="54" x14ac:dyDescent="0.15">
+      <c r="A7" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A8" s="6" t="s">
+      <c r="C7" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="D7" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="36" x14ac:dyDescent="0.15">
+      <c r="A8" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.15">
-      <c r="A9" s="6" t="s">
+      <c r="C8" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="D8" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.15">
-      <c r="A10" s="6" t="s">
+      <c r="C9" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D9" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.15">
+      <c r="A10" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A11" s="6" t="s">
+      <c r="C10" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D10" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="36" x14ac:dyDescent="0.15">
+      <c r="A11" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="72" x14ac:dyDescent="0.15">
-      <c r="A12" s="6" t="s">
+      <c r="C11" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D11" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D12" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="36" x14ac:dyDescent="0.15">
+      <c r="A13" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D13" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="72" x14ac:dyDescent="0.15">
+      <c r="A14" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D14" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="54" x14ac:dyDescent="0.15">
+      <c r="A15" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="D15" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="36" x14ac:dyDescent="0.15">
+      <c r="A16" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="72" x14ac:dyDescent="0.15">
-      <c r="A14" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="54" x14ac:dyDescent="0.15">
-      <c r="A15" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A16" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="B16" s="4" t="s">
+      <c r="C16" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="D16" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="54" x14ac:dyDescent="0.15">
+      <c r="A17" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="54" x14ac:dyDescent="0.15">
-      <c r="A17" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="126" x14ac:dyDescent="0.15">
-      <c r="A18" s="6" t="s">
+      <c r="C17" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="D17" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="126" x14ac:dyDescent="0.15">
+      <c r="A18" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A19" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="D18" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="36" x14ac:dyDescent="0.15">
+      <c r="A19" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A20" s="4" t="s">
+      <c r="C19" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="D19" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="36" x14ac:dyDescent="0.15">
+      <c r="A20" s="10" t="s">
         <v>27</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A21" s="4" t="s">
+      <c r="C20" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="D20" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="36" x14ac:dyDescent="0.15">
+      <c r="A21" s="10" t="s">
         <v>29</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A22" s="4" t="s">
+      <c r="C21" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="D21" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="36" x14ac:dyDescent="0.15">
+      <c r="A22" s="10" t="s">
         <v>31</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="54" x14ac:dyDescent="0.15">
-      <c r="A23" s="6" t="s">
+      <c r="C22" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D22" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="54" x14ac:dyDescent="0.15">
+      <c r="A23" s="10" t="s">
         <v>33</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A24" s="9" t="s">
+      <c r="C23" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="D23" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="36" x14ac:dyDescent="0.15">
+      <c r="A24" s="10" t="s">
         <v>35</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A25" s="9" t="s">
+      <c r="C24" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="D24" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="36" x14ac:dyDescent="0.15">
+      <c r="A25" s="10" t="s">
         <v>37</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="18" x14ac:dyDescent="0.15">
-      <c r="A26" s="4" t="s">
+      <c r="C25" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D25" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="18" x14ac:dyDescent="0.15">
+      <c r="A26" s="10" t="s">
         <v>39</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A27" s="6" t="s">
+      <c r="C26" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="D26" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="36" x14ac:dyDescent="0.15">
+      <c r="A27" s="10" t="s">
         <v>41</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A28" s="6" t="s">
+      <c r="C27" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D27" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="36" x14ac:dyDescent="0.15">
+      <c r="A28" s="10" t="s">
         <v>43</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="18" x14ac:dyDescent="0.15">
-      <c r="A29" s="4" t="s">
+      <c r="C28" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D28" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="18" x14ac:dyDescent="0.15">
+      <c r="A29" s="10" t="s">
         <v>45</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A30" s="6" t="s">
+      <c r="C29" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="D29" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="36" x14ac:dyDescent="0.15">
+      <c r="A30" s="10" t="s">
         <v>47</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="18" x14ac:dyDescent="0.15">
-      <c r="A31" s="6" t="s">
+      <c r="C30" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D30" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="18" x14ac:dyDescent="0.15">
+      <c r="A31" s="10" t="s">
         <v>49</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A32" s="6" t="s">
+      <c r="C31" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D31" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="36" x14ac:dyDescent="0.15">
+      <c r="A32" s="10" t="s">
         <v>51</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A33" s="6" t="s">
+      <c r="C32" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D32" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="36" x14ac:dyDescent="0.15">
+      <c r="A33" s="10" t="s">
         <v>53</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A34" s="6" t="s">
+      <c r="C33" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D33" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="36" x14ac:dyDescent="0.15">
+      <c r="A34" s="10" t="s">
         <v>55</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A35" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D34" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="36" x14ac:dyDescent="0.15">
+      <c r="A35" s="10" t="s">
         <v>56</v>
       </c>
       <c r="B35" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D35" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="18" x14ac:dyDescent="0.15">
+      <c r="A36" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D36" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="36" x14ac:dyDescent="0.15">
+      <c r="A37" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="7" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="18" x14ac:dyDescent="0.15">
-      <c r="A36" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A37" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="18" x14ac:dyDescent="0.15">
-      <c r="A38" s="7" t="s">
+      <c r="C37" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D37" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="18" x14ac:dyDescent="0.15">
+      <c r="A38" s="11" t="s">
         <v>59</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A39" s="7" t="s">
+      <c r="C38" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D38" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="36" x14ac:dyDescent="0.15">
+      <c r="A39" s="11" t="s">
         <v>61</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A40" s="4" t="s">
+      <c r="C39" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D39" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="36" x14ac:dyDescent="0.15">
+      <c r="A40" s="10" t="s">
         <v>63</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A41" s="4" t="s">
+      <c r="C40" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D40" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="36" x14ac:dyDescent="0.15">
+      <c r="A41" s="10" t="s">
         <v>65</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" ht="18" x14ac:dyDescent="0.15">
-      <c r="A42" s="6" t="s">
+      <c r="C41" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D41" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="18" x14ac:dyDescent="0.15">
+      <c r="A42" s="10" t="s">
         <v>67</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A43" s="6" t="s">
+      <c r="C42" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D42" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="36" x14ac:dyDescent="0.15">
+      <c r="A43" s="10" t="s">
         <v>69</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A44" s="6" t="s">
+      <c r="C43" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D43" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="36" x14ac:dyDescent="0.15">
+      <c r="A44" s="10" t="s">
         <v>71</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A45" s="6" t="s">
+      <c r="C44" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D44" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="36" x14ac:dyDescent="0.15">
+      <c r="A45" s="10" t="s">
         <v>73</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A46" s="6" t="s">
+      <c r="C45" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D45" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="36" x14ac:dyDescent="0.15">
+      <c r="A46" s="10" t="s">
         <v>75</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A47" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D46" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="36" x14ac:dyDescent="0.15">
+      <c r="A47" s="10" t="s">
         <v>76</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" ht="72" x14ac:dyDescent="0.15">
-      <c r="A48" s="4" t="s">
+      <c r="C47" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D47" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="72" x14ac:dyDescent="0.15">
+      <c r="A48" s="10" t="s">
         <v>78</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" ht="18" x14ac:dyDescent="0.15">
-      <c r="A49" s="4" t="s">
+      <c r="C48" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D48" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="18" x14ac:dyDescent="0.15">
+      <c r="A49" s="10" t="s">
         <v>80</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A50" s="4" t="s">
+      <c r="C49" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="D49" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="36" x14ac:dyDescent="0.15">
+      <c r="A50" s="10" t="s">
         <v>82</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A51" s="4" t="s">
-        <v>159</v>
+      <c r="C50" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="D50" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="36" x14ac:dyDescent="0.15">
+      <c r="A51" s="10" t="s">
+        <v>157</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" ht="18" x14ac:dyDescent="0.15">
-      <c r="A52" s="4" t="s">
+      <c r="C51" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D51" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="18" x14ac:dyDescent="0.15">
+      <c r="A52" s="10" t="s">
         <v>85</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A53" s="4" t="s">
+      <c r="C52" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D52" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="36" x14ac:dyDescent="0.15">
+      <c r="A53" s="10" t="s">
         <v>87</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" ht="54" x14ac:dyDescent="0.15">
-      <c r="A54" s="4" t="s">
+      <c r="C53" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D53" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="54" x14ac:dyDescent="0.15">
+      <c r="A54" s="10" t="s">
         <v>89</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" ht="54" x14ac:dyDescent="0.15">
-      <c r="A55" s="4" t="s">
+      <c r="C54" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D54" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="54" x14ac:dyDescent="0.15">
+      <c r="A55" s="10" t="s">
         <v>91</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" ht="54" x14ac:dyDescent="0.15">
-      <c r="A56" s="4" t="s">
+      <c r="C55" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D55" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="54" x14ac:dyDescent="0.15">
+      <c r="A56" s="10" t="s">
         <v>93</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" ht="54" x14ac:dyDescent="0.15">
-      <c r="A57" s="4" t="s">
+      <c r="C56" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D56" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="54" x14ac:dyDescent="0.15">
+      <c r="A57" s="10" t="s">
         <v>95</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A58" s="4" t="s">
+      <c r="C57" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D57" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="36" x14ac:dyDescent="0.15">
+      <c r="A58" s="10" t="s">
         <v>97</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A59" s="4" t="s">
+      <c r="C58" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D58" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="36" x14ac:dyDescent="0.15">
+      <c r="A59" s="10" t="s">
         <v>99</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" ht="54" x14ac:dyDescent="0.15">
-      <c r="A60" s="6" t="s">
+      <c r="C59" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D59" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="54" x14ac:dyDescent="0.15">
+      <c r="A60" s="10" t="s">
         <v>101</v>
       </c>
       <c r="B60" s="6" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" ht="18" x14ac:dyDescent="0.15">
-      <c r="A61" s="4" t="s">
+      <c r="C60" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D60" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="18" x14ac:dyDescent="0.15">
+      <c r="A61" s="10" t="s">
         <v>103</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A62" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D61" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="36" x14ac:dyDescent="0.15">
+      <c r="A62" s="10" t="s">
         <v>104</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="18" x14ac:dyDescent="0.15">
-      <c r="A63" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D62" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="18" x14ac:dyDescent="0.15">
+      <c r="A63" s="10" t="s">
         <v>105</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" ht="18" x14ac:dyDescent="0.15">
-      <c r="A64" s="4" t="s">
+      <c r="C63" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D63" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="18" x14ac:dyDescent="0.15">
+      <c r="A64" s="10" t="s">
         <v>107</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" ht="18" x14ac:dyDescent="0.15">
-      <c r="A65" s="4" t="s">
+      <c r="C64" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D64" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="18" x14ac:dyDescent="0.15">
+      <c r="A65" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B65" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="C65" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D65" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="18" x14ac:dyDescent="0.15">
+      <c r="A66" s="10" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" ht="18" x14ac:dyDescent="0.15">
-      <c r="A66" s="4" t="s">
+      <c r="B66" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="C66" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="D66" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="18" x14ac:dyDescent="0.15">
+      <c r="A67" s="10" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" ht="18" x14ac:dyDescent="0.15">
-      <c r="A67" s="4" t="s">
+      <c r="B67" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="C67" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D67" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="36" x14ac:dyDescent="0.15">
+      <c r="A68" s="10" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A68" s="6" t="s">
+      <c r="B68" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="C68" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D68" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="18" x14ac:dyDescent="0.15">
+      <c r="A69" s="10" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" ht="18" x14ac:dyDescent="0.15">
-      <c r="A69" s="4" t="s">
+      <c r="B69" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="C69" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D69" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="54" x14ac:dyDescent="0.15">
+      <c r="A70" s="10" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" ht="54" x14ac:dyDescent="0.15">
-      <c r="A70" s="4" t="s">
+      <c r="B70" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D70" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="54" x14ac:dyDescent="0.15">
+      <c r="A71" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="B70" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="54" x14ac:dyDescent="0.15">
-      <c r="A71" s="4" t="s">
+      <c r="B71" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="C71" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D71" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="36" x14ac:dyDescent="0.15">
+      <c r="A72" s="10" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A72" s="4" t="s">
+      <c r="B72" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="C72" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D72" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="36" x14ac:dyDescent="0.15">
+      <c r="A73" s="10" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A73" s="4" t="s">
+      <c r="B73" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="C73" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D73" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="36" x14ac:dyDescent="0.15">
+      <c r="A74" s="10" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A74" s="4" t="s">
+      <c r="B74" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="C74" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D74" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="18" x14ac:dyDescent="0.15">
+      <c r="A75" s="10" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" ht="18" x14ac:dyDescent="0.15">
-      <c r="A75" s="4" t="s">
+      <c r="B75" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="C75" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D75" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="18" x14ac:dyDescent="0.15">
+      <c r="A76" s="10" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" ht="18" x14ac:dyDescent="0.15">
-      <c r="A76" s="4" t="s">
+      <c r="B76" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="C76" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D76" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="54" x14ac:dyDescent="0.15">
+      <c r="A77" s="10" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" ht="54" x14ac:dyDescent="0.15">
-      <c r="A77" s="4" t="s">
+      <c r="B77" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="C77" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D77" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="18" x14ac:dyDescent="0.15">
+      <c r="A78" s="10" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" ht="18" x14ac:dyDescent="0.15">
-      <c r="A78" s="4" t="s">
+      <c r="B78" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="C78" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D78" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="36" x14ac:dyDescent="0.15">
+      <c r="A79" s="10" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" ht="36" x14ac:dyDescent="0.15">
-      <c r="A79" s="4" t="s">
+      <c r="B79" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="C79" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D79" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="18" x14ac:dyDescent="0.15">
+      <c r="A80" s="10" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" ht="18" x14ac:dyDescent="0.15">
-      <c r="A80" s="4" t="s">
+      <c r="B80" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="C80" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D80" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="18" x14ac:dyDescent="0.15">
+      <c r="A81" s="10" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" ht="18" x14ac:dyDescent="0.15">
-      <c r="A81" s="4" t="s">
+      <c r="B81" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="C81" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D81" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="18" x14ac:dyDescent="0.15">
+      <c r="A82" s="10" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" ht="18" x14ac:dyDescent="0.15">
-      <c r="A82" s="4" t="s">
+      <c r="B82" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B82" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A83" s="1"/>
+      <c r="C82" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D82" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A83" s="13"/>
       <c r="B83" s="1"/>
     </row>
-    <row r="84" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A84" s="1"/>
+    <row r="84" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A84" s="13"/>
       <c r="B84" s="1"/>
     </row>
-    <row r="85" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A85" s="1"/>
+    <row r="85" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A85" s="13"/>
       <c r="B85" s="1"/>
     </row>
-    <row r="86" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A86" s="1"/>
+    <row r="86" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A86" s="13"/>
       <c r="B86" s="1"/>
     </row>
-    <row r="87" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A87" s="1"/>
+    <row r="87" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A87" s="13"/>
       <c r="B87" s="1"/>
     </row>
-    <row r="88" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A88" s="1"/>
+    <row r="88" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A88" s="13"/>
       <c r="B88" s="1"/>
     </row>
-    <row r="89" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A89" s="1"/>
+    <row r="89" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A89" s="13"/>
       <c r="B89" s="1"/>
     </row>
-    <row r="90" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A90" s="1"/>
+    <row r="90" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A90" s="13"/>
       <c r="B90" s="1"/>
     </row>
-    <row r="91" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A91" s="1"/>
+    <row r="91" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A91" s="13"/>
       <c r="B91" s="1"/>
     </row>
-    <row r="92" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A92" s="1"/>
+    <row r="92" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A92" s="13"/>
       <c r="B92" s="1"/>
     </row>
-    <row r="93" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A93" s="1"/>
+    <row r="93" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A93" s="13"/>
       <c r="B93" s="1"/>
     </row>
-    <row r="94" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A94" s="1"/>
+    <row r="94" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A94" s="13"/>
       <c r="B94" s="1"/>
     </row>
-    <row r="95" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A95" s="1"/>
+    <row r="95" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A95" s="13"/>
       <c r="B95" s="1"/>
     </row>
-    <row r="96" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A96" s="1"/>
+    <row r="96" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A96" s="13"/>
       <c r="B96" s="1"/>
     </row>
     <row r="97" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A97" s="1"/>
+      <c r="A97" s="13"/>
       <c r="B97" s="1"/>
     </row>
     <row r="98" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A98" s="1"/>
+      <c r="A98" s="13"/>
       <c r="B98" s="1"/>
     </row>
     <row r="99" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A99" s="1"/>
+      <c r="A99" s="13"/>
       <c r="B99" s="1"/>
     </row>
     <row r="100" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A100" s="1"/>
+      <c r="A100" s="13"/>
       <c r="B100" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="C1:C100"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" scale="71" pageOrder="overThenDown" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <colBreaks count="1" manualBreakCount="1">
-    <brk id="2" max="1048575" man="1"/>
+    <brk id="4" max="1048575" man="1"/>
   </colBreaks>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change some format of Data-VAriable-Definitions.xlsx
</commit_message>
<xml_diff>
--- a/ref/Data-Variable-Definitions.xlsx
+++ b/ref/Data-Variable-Definitions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xiaoba/Projects/Udacity/dand-p4-explore-summarise-data/ref/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xiaoba/Projects/Udacity/prosper-loan/ref/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -840,19 +840,19 @@
     </xf>
   </cellXfs>
   <cellStyles count="13">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1129,9 +1129,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1245,7 +1245,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="54" x14ac:dyDescent="0.15">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -2048,7 +2048,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" ht="36" x14ac:dyDescent="0.15">
-      <c r="A62" s="10" t="s">
+      <c r="A62" s="6" t="s">
         <v>104</v>
       </c>
       <c r="B62" s="4" t="s">

</xml_diff>